<commit_message>
Update .gitignore, refactor slides script and improve slide-change handling
Added a new rule in .gitignore file to ignore specific desktop.ini file. The scripts for the slides-v1.js file were cleaned up, particularly in the grammar of the robot's speech, typographical errors in the filenames, and replacing some redundant code constructs with a reusable function. In the presentationCtrl.js, a function for safely setting the slide index was introduced, protecting against potential index-out-of-bounds errors and encapsulating the action of storing the index in local storage.
</commit_message>
<xml_diff>
--- a/docs/images/exclusion-chart.xlsx
+++ b/docs/images/exclusion-chart.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\code\decentralized-fda\docs\images\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2DDD93E1-7728-475C-839E-64AED4D956F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{283C62CD-FCB2-4EDB-B887-68AA126A753B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="22149" windowHeight="13200" xr2:uid="{F5C99788-4B1A-42E1-8DBE-14AA78FEBFDA}"/>
   </bookViews>
@@ -249,8 +249,8 @@
               <c:idx val="0"/>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-0.17999192042402085"/>
-                  <c:y val="0.26397820997445071"/>
+                  <c:x val="-0.17065236202579684"/>
+                  <c:y val="0.25828715324604207"/>
                 </c:manualLayout>
               </c:layout>
               <c:tx>
@@ -501,12 +501,9 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="2400" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="85000"/>
-                        <a:lumOff val="15000"/>
-                      </a:schemeClr>
+                      <a:schemeClr val="accent1"/>
                     </a:solidFill>
                     <a:latin typeface="+mn-lt"/>
                     <a:ea typeface="+mn-ea"/>
@@ -516,27 +513,12 @@
                 <a:endParaRPr lang="en-US"/>
               </a:p>
             </c:txPr>
-            <c:dLblPos val="inEnd"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
-            <c:showCatName val="1"/>
+            <c:showCatName val="0"/>
             <c:showSerName val="0"/>
-            <c:showPercent val="1"/>
+            <c:showPercent val="0"/>
             <c:showBubbleSize val="0"/>
-            <c:showLeaderLines val="1"/>
-            <c:leaderLines>
-              <c:spPr>
-                <a:ln w="9525">
-                  <a:solidFill>
-                    <a:schemeClr val="accent1">
-                      <a:lumMod val="60000"/>
-                      <a:lumOff val="40000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                </a:ln>
-                <a:effectLst/>
-              </c:spPr>
-            </c:leaderLines>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
             </c:extLst>
@@ -1565,7 +1547,7 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N18" sqref="N18"/>
+      <selection activeCell="N10" sqref="N10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>

</xml_diff>